<commit_message>
Final analysis for draft
</commit_message>
<xml_diff>
--- a/Social charging model/SCM_export_results_sensitivity.xlsx
+++ b/Social charging model/SCM_export_results_sensitivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naudl\Documents\GitHub\social-charging-model\Social charging model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABD338-318F-4A13-A525-A25B5EAD158B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1BAD60-64BA-4779-B48C-CA81067C2B56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{3758AFA0-8E81-488E-A41A-47B84DA45D8A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{3758AFA0-8E81-488E-A41A-47B84DA45D8A}"/>
   </bookViews>
   <sheets>
     <sheet name="per_timestep" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>scenario</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>rcs</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>trips</t>
+  </si>
+  <si>
+    <t>kmd</t>
   </si>
 </sst>
 </file>
@@ -468,15 +477,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C276F534-E875-46ED-80D0-6FDBCE465A6B}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD364001"/>
+      <selection activeCell="A2" sqref="A2:L51949"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,7 +493,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -506,6 +515,12 @@
       </c>
       <c r="J1" t="s">
         <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>